<commit_message>
export csv all orders of customer at once it will not export select orders -yet to do this
</commit_message>
<xml_diff>
--- a/accounts/excel/Demo_excel.xlsx
+++ b/accounts/excel/Demo_excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1920" yWindow="1320" windowWidth="15375" windowHeight="7875" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Duration_calculator" sheetId="1" state="visible" r:id="rId1"/>
@@ -428,10 +428,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -486,6 +486,21 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>44486</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>URC-2021-12-19</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>9W</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>